<commit_message>
Remaining distance to keep current status added to Excel
</commit_message>
<xml_diff>
--- a/DriveTemplateDevelopment.xlsx
+++ b/DriveTemplateDevelopment.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFCCA88-6ACB-4BFA-BED9-017C3AB0E509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7269803-218D-4718-B04F-3CDC29A5C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Discovery Drive" sheetId="2" r:id="rId1"/>
-    <sheet name="Drive" sheetId="4" r:id="rId2"/>
+    <sheet name="Christiaan" sheetId="5" r:id="rId2"/>
+    <sheet name="Develop" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>End</t>
   </si>
@@ -141,10 +164,53 @@
     <t>The predicted status gives a more realistic prediction of the driving status. If the rediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
   </si>
   <si>
-    <t>Stefan</t>
-  </si>
-  <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Bracket</t>
+  </si>
+  <si>
+    <t>Distance Brackets</t>
+  </si>
+  <si>
+    <t>Driving Status</t>
+  </si>
+  <si>
+    <t>Lowlim</t>
+  </si>
+  <si>
+    <t>CurrPt</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>20 times</t>
+  </si>
+  <si>
+    <t>New Brack</t>
+  </si>
+  <si>
+    <t>xlook</t>
+  </si>
+  <si>
+    <t>Rem dis</t>
+  </si>
+  <si>
+    <t>min ektra</t>
+  </si>
+  <si>
+    <t>Daily Average</t>
+  </si>
+  <si>
+    <t>The predicted status gives a more realistic prediction of the driving status. 
+If the rediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
   </si>
 </sst>
 </file>
@@ -292,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,26 +455,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,12 +819,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEDDE97-743E-47DB-AEB3-A3993515C83A}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:H30"/>
     </sheetView>
   </sheetViews>
@@ -771,17 +848,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="N1" s="35" t="s">
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="N1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1662,10 +1739,10 @@
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="18">
         <f>SUM(G3:G33)</f>
         <v>1613.018</v>
@@ -1725,38 +1802,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE70C601-B43B-41C4-8E7C-4A1600D76DAD}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75474B4D-967A-4F20-BCE0-BD3D1E7287B1}">
+  <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:S50"/>
+  <dimension ref="B2:V50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.42578125" style="6" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="9.42578125" style="6" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="5" style="17" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="6"/>
+    <col min="13" max="13" width="9.42578125" style="17" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="9.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="18" width="8.85546875" style="6"/>
+    <col min="19" max="19" width="8.85546875" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="str">
-        <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan August 2024</v>
+    <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="38" t="str" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">_xlfn.CONCAT("Drive Summary ", MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,31), " ",TEXT(TODAY(), "mmmm yyyy"))</f>
+        <v>Drive Summary Christiaan August 2024</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
@@ -1764,7 +1841,7 @@
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
     </row>
-    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
@@ -1772,13 +1849,13 @@
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="25">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>1500</v>
+        <v>850</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
@@ -1786,39 +1863,35 @@
         <v>August 2024</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="34"/>
-      <c r="M5" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I5" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="K5" s="35"/>
+      <c r="M5" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="35"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="23">
-        <v>300</v>
-      </c>
+      <c r="C6" s="23"/>
       <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="30">
-        <v>1533.018</v>
-      </c>
-      <c r="G6" s="23">
-        <v>1381</v>
-      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="23"/>
       <c r="I6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1829,10 +1902,10 @@
         <v>17</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>15</v>
@@ -1840,25 +1913,26 @@
       <c r="P6" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T6"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="23">
-        <v>300</v>
-      </c>
+      <c r="C7" s="23"/>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="25">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>6789.0797142857145</v>
+        <v>0</v>
       </c>
       <c r="G7" s="25">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>6115.8571428571422</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1881,14 +1955,15 @@
       <c r="P7" s="12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="U7" s="41"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="1"/>
@@ -1914,21 +1989,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="23">
-        <v>300</v>
-      </c>
+      <c r="C9" s="23"/>
       <c r="E9" s="7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I9" s="1">
         <v>300</v>
@@ -1953,24 +2026,24 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2500</v>
+        <v>1150</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="24">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>219.00257142857143</v>
+        <v>0</v>
       </c>
       <c r="G10" s="24">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>197.28571428571428</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -1994,7 +2067,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -2016,19 +2089,20 @@
       <c r="P11" s="12">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S11"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
-        <v>Diamond</v>
+        <v>Bronze</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="26"/>
       <c r="F12" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>17</v>
@@ -2043,25 +2117,23 @@
         <v>200</v>
       </c>
       <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="33"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="13">
-        <f>0</f>
-        <v>0</v>
-      </c>
+      <c r="C13" s="44"/>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F13" s="25">
-        <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
-        <v>115.98199999999997</v>
+        <f ca="1">IF(INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)=0,0,INT((C10-VLOOKUP(C10,M7:O11,1,TRUE))/20)*150-1)+(VLOOKUP(F6,I7:K21,2,TRUE)-F6)</f>
+        <v>2698</v>
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>1200</v>
+        <v>850</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2072,18 +2144,16 @@
       <c r="K13" s="1">
         <v>180</v>
       </c>
-      <c r="M13" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="37"/>
-      <c r="O13"/>
-      <c r="P13"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="9"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="8">
         <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
         <v>0</v>
       </c>
@@ -2101,9 +2171,8 @@
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D15" s="14"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -2116,11 +2185,13 @@
       </c>
       <c r="M15"/>
       <c r="N15"/>
-      <c r="O15"/>
+      <c r="O15" s="43"/>
       <c r="P15"/>
       <c r="Q15"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -2138,13 +2209,12 @@
       </c>
       <c r="M16"/>
       <c r="N16"/>
-      <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="39" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -2166,7 +2236,7 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -2188,7 +2258,7 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -2210,7 +2280,7 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -2231,15 +2301,15 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="I21" s="1">
         <v>2100</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>0</v>
+      <c r="J21" s="1">
+        <v>2100</v>
       </c>
       <c r="K21" s="1">
         <v>20</v>
@@ -2249,14 +2319,18 @@
       <c r="O21"/>
       <c r="P21"/>
       <c r="Q21"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="Q22"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -2264,49 +2338,49 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="21"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="21"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E32" s="26"/>
       <c r="F32" s="28"/>
       <c r="G32" s="27"/>
@@ -2394,9 +2468,796 @@
       <c r="M50" s="6"/>
     </row>
   </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput"/>
+  </protectedRanges>
   <mergeCells count="5">
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="I5:K5"/>
     <mergeCell ref="M5:P5"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="B17:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE70C601-B43B-41C4-8E7C-4A1600D76DAD}">
+  <sheetPr codeName="Sheet2">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:V50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8.85546875" style="6"/>
+    <col min="19" max="19" width="8.85546875" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="38" t="str" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">_xlfn.CONCAT("Drive Summary ", MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,31), " ",TEXT(TODAY(), "mmmm yyyy"))</f>
+        <v>Drive Summary Develop August 2024</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="25">
+        <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
+        <v>1500</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="7" t="str">
+        <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
+        <v>August 2024</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="K5" s="35"/>
+      <c r="M5" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="35"/>
+      <c r="U5" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="42"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="23">
+        <v>150</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="30">
+        <v>354</v>
+      </c>
+      <c r="G6" s="23">
+        <v>698</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="V6" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="23">
+        <v>330</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="25">
+        <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
+        <v>783.85714285714278</v>
+      </c>
+      <c r="G7" s="25">
+        <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
+        <v>1545.5714285714284</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>149</v>
+      </c>
+      <c r="K7" s="1">
+        <v>300</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>799</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="6">
+        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
+        <v>850</v>
+      </c>
+      <c r="U7" s="41">
+        <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
+        <v>260</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1">
+        <v>150</v>
+      </c>
+      <c r="J8" s="1">
+        <v>299</v>
+      </c>
+      <c r="K8" s="1">
+        <v>280</v>
+      </c>
+      <c r="M8" s="1">
+        <v>800</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1599</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="23">
+        <v>300</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>300</v>
+      </c>
+      <c r="J9" s="1">
+        <v>449</v>
+      </c>
+      <c r="K9" s="1">
+        <v>260</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1600</v>
+      </c>
+      <c r="N9" s="1">
+        <v>2199</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="R9" s="9"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8">
+        <f ca="1">SUM(C5:C9)</f>
+        <v>2540</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="24">
+        <f ca="1">F6/(DAY(TODAY())-1)</f>
+        <v>25.285714285714285</v>
+      </c>
+      <c r="G10" s="24">
+        <f ca="1">G6/(DAY(TODAY())-1)</f>
+        <v>49.857142857142854</v>
+      </c>
+      <c r="I10" s="1">
+        <v>450</v>
+      </c>
+      <c r="J10" s="1">
+        <v>599</v>
+      </c>
+      <c r="K10" s="1">
+        <v>240</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2200</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2499</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="6" t="str">
+        <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
+        <v>Diamond</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>600</v>
+      </c>
+      <c r="J11" s="1">
+        <v>749</v>
+      </c>
+      <c r="K11" s="1">
+        <v>220</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2500</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3000</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="S11"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
+        <v>Diamond</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1">
+        <v>750</v>
+      </c>
+      <c r="J12" s="1">
+        <v>899</v>
+      </c>
+      <c r="K12" s="1">
+        <v>200</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="S12" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="T12" s="6">
+        <f ca="1">VLOOKUP(C10,M7:O11,1,TRUE)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="25">
+        <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
+        <v>95</v>
+      </c>
+      <c r="G13" s="1">
+        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
+        <v>850</v>
+      </c>
+      <c r="I13" s="1">
+        <v>900</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1049</v>
+      </c>
+      <c r="K13" s="1">
+        <v>180</v>
+      </c>
+      <c r="N13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="S13" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="T13" s="9">
+        <f ca="1">C5+C6+C7+C9+C8</f>
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1050</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1199</v>
+      </c>
+      <c r="K14" s="1">
+        <v>160</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D15" s="14"/>
+      <c r="I15" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1349</v>
+      </c>
+      <c r="K15" s="1">
+        <v>140</v>
+      </c>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="S15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T15" s="9">
+        <f ca="1">T13-T12</f>
+        <v>40</v>
+      </c>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1350</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1499</v>
+      </c>
+      <c r="K16" s="1">
+        <v>120</v>
+      </c>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="S16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T16" s="6">
+        <f ca="1">INT(T15/20)</f>
+        <v>2</v>
+      </c>
+      <c r="U16" s="6">
+        <f ca="1">IF(T16=0,0,T16*150-1)</f>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="I17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1649</v>
+      </c>
+      <c r="K17" s="1">
+        <v>100</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="S17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T17" s="6">
+        <f ca="1">20*T16</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="I18" s="1">
+        <v>1650</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1799</v>
+      </c>
+      <c r="K18" s="1">
+        <v>80</v>
+      </c>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="S18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="6">
+        <f ca="1">MIN(300-T17,C8)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="I19" s="1">
+        <v>1800</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1949</v>
+      </c>
+      <c r="K19" s="1">
+        <v>60</v>
+      </c>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="S19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T19" s="6">
+        <f ca="1">_xlfn.XLOOKUP(T18,K7:K21,J7:J21)</f>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="I20" s="1">
+        <v>1950</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2099</v>
+      </c>
+      <c r="K20" s="1">
+        <v>40</v>
+      </c>
+      <c r="M20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="I21" s="1">
+        <v>2100</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2100</v>
+      </c>
+      <c r="K21" s="1">
+        <v>20</v>
+      </c>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="S21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T21" s="9">
+        <f ca="1">T19-F6</f>
+        <v>95</v>
+      </c>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="Q22"/>
+      <c r="S22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="T22" s="9">
+        <f ca="1">T21-F13</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24" s="21"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25" s="21"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M27" s="6"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M28" s="6"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="J29" s="4"/>
+      <c r="M29" s="6"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M30" s="6"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
+      <c r="M31" s="6"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E32" s="26"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="27"/>
+      <c r="M32" s="6"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="26"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="27"/>
+      <c r="M33" s="6"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E34" s="26"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="27"/>
+      <c r="K34" s="3"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E35" s="26"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="27"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E36" s="26"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="27"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E37" s="26"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="27"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E38" s="26"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="27"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E39" s="26"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H41" s="19"/>
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="M42" s="6"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M43" s="6"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I44" s="3"/>
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M45" s="6"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="M5:P5"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="B17:G19"/>
     <mergeCell ref="I5:K5"/>

</xml_diff>